<commit_message>
It compiles. But doesn't work. Woot.
</commit_message>
<xml_diff>
--- a/MatchAnalysis/DataFiles/ESupers_Hopper_Match_Results.xlsx
+++ b/MatchAnalysis/DataFiles/ESupers_Hopper_Match_Results.xlsx
@@ -430,7 +430,7 @@
   <dimension ref="A1:G82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,7 +570,7 @@
         <v>5017</v>
       </c>
       <c r="D6">
-        <v>7717</v>
+        <v>7117</v>
       </c>
       <c r="E6">
         <v>8619</v>

</xml_diff>